<commit_message>
Added ContentBuilder solution to the repo. ContentBuilder now compiles shaders for Xbox, WiiU, PS3, and PC-C++.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -3009,52 +3009,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3103,13 +3062,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3413,8 +3365,8 @@
   <dimension ref="A1:J800"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J307" sqref="J307"/>
+      <pane ySplit="1" topLeftCell="A768" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J305" sqref="J305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10115,7 +10067,7 @@
         <v>738</v>
       </c>
       <c r="D210" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>1</v>
@@ -11290,7 +11242,7 @@
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>1</v>
@@ -13146,7 +13098,7 @@
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>1</v>
@@ -13155,7 +13107,7 @@
         <v>738</v>
       </c>
       <c r="D305" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="E305" s="1" t="s">
         <v>1</v>
@@ -13164,7 +13116,7 @@
         <v>738</v>
       </c>
       <c r="G305" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="H305" s="1" t="s">
         <v>1</v>
@@ -13178,7 +13130,7 @@
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B306" s="1" t="s">
         <v>1</v>
@@ -13187,7 +13139,7 @@
         <v>738</v>
       </c>
       <c r="D306" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="E306" s="1" t="s">
         <v>1</v>
@@ -13196,7 +13148,7 @@
         <v>738</v>
       </c>
       <c r="G306" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="H306" s="1" t="s">
         <v>1</v>
@@ -26842,7 +26794,7 @@
     </row>
     <row r="733" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A733" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B733" s="1" t="s">
         <v>1</v>
@@ -26851,7 +26803,7 @@
         <v>738</v>
       </c>
       <c r="D733" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="E733" s="1" t="s">
         <v>1</v>
@@ -26860,7 +26812,7 @@
         <v>738</v>
       </c>
       <c r="G733" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="H733" s="1" t="s">
         <v>1</v>
@@ -29020,30 +28972,30 @@
   <sortState ref="A2:J800">
     <sortCondition ref="J2:J800"/>
   </sortState>
-  <conditionalFormatting sqref="A2:J734 A735:I800">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+  <conditionalFormatting sqref="A735:I800 A2:J734">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576 I1:I1048576 F1:F1048576">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576 E1:E1048576 B1:B1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29056,7 +29008,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576 A2:A1048576 G2:G1048576</xm:sqref>
+          <xm:sqref>G2:G1048576 D2:D1048576 A2:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Added Translation Master.xlsx, which is converted to a .tsv file on build.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -3785,8 +3785,8 @@
   <dimension ref="A1:Q800"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P26" sqref="P26"/>
+      <pane ySplit="1" topLeftCell="A768" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H786" sqref="H786"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45399,7 +45399,7 @@
         <v>814</v>
       </c>
       <c r="B786" s="13" t="s">
-        <v>814</v>
+        <v>736</v>
       </c>
       <c r="C786" s="13" t="s">
         <v>814</v>
@@ -45435,7 +45435,7 @@
         <v>0</v>
       </c>
       <c r="N786" s="1" t="s">
-        <v>815</v>
+        <v>1</v>
       </c>
       <c r="O786" s="1" t="s">
         <v>738</v>
@@ -45452,7 +45452,7 @@
         <v>814</v>
       </c>
       <c r="B787" s="13" t="s">
-        <v>814</v>
+        <v>736</v>
       </c>
       <c r="C787" s="13" t="s">
         <v>814</v>
@@ -45461,7 +45461,7 @@
         <v>814</v>
       </c>
       <c r="E787" s="13" t="s">
-        <v>814</v>
+        <v>739</v>
       </c>
       <c r="F787" s="13" t="s">
         <v>814</v>
@@ -45488,7 +45488,7 @@
         <v>0</v>
       </c>
       <c r="N787" s="1" t="s">
-        <v>815</v>
+        <v>1</v>
       </c>
       <c r="O787" s="1" t="s">
         <v>738</v>

</xml_diff>

<commit_message>
New hero unlocked message added.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13603" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13620" uniqueCount="818">
   <si>
     <t>Include</t>
   </si>
@@ -2466,6 +2466,9 @@
   </si>
   <si>
     <t>Video Memory</t>
+  </si>
+  <si>
+    <t>Art/Title/Categories/Arcade/MessageBoxThin</t>
   </si>
 </sst>
 </file>
@@ -3080,11 +3083,204 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="75">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3782,11 +3978,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q800"/>
+  <dimension ref="A1:Q801"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A768" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H786" sqref="H786"/>
+      <pane ySplit="1" topLeftCell="A767" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P789" sqref="P789"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45387,7 +45583,7 @@
       <c r="O785" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="P785" s="7" t="s">
+      <c r="P785" s="6" t="s">
         <v>719</v>
       </c>
       <c r="Q785" s="5" t="s">
@@ -45399,7 +45595,7 @@
         <v>814</v>
       </c>
       <c r="B786" s="13" t="s">
-        <v>736</v>
+        <v>814</v>
       </c>
       <c r="C786" s="13" t="s">
         <v>814</v>
@@ -45435,13 +45631,13 @@
         <v>0</v>
       </c>
       <c r="N786" s="1" t="s">
-        <v>1</v>
+        <v>741</v>
       </c>
       <c r="O786" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="P786" s="7" t="s">
-        <v>720</v>
+      <c r="P786" s="6" t="s">
+        <v>817</v>
       </c>
       <c r="Q786" s="5" t="s">
         <v>738</v>
@@ -45461,7 +45657,7 @@
         <v>814</v>
       </c>
       <c r="E787" s="13" t="s">
-        <v>739</v>
+        <v>814</v>
       </c>
       <c r="F787" s="13" t="s">
         <v>814</v>
@@ -45494,7 +45690,7 @@
         <v>738</v>
       </c>
       <c r="P787" s="7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="Q787" s="5" t="s">
         <v>738</v>
@@ -45505,7 +45701,7 @@
         <v>814</v>
       </c>
       <c r="B788" s="13" t="s">
-        <v>814</v>
+        <v>736</v>
       </c>
       <c r="C788" s="13" t="s">
         <v>814</v>
@@ -45514,7 +45710,7 @@
         <v>814</v>
       </c>
       <c r="E788" s="13" t="s">
-        <v>814</v>
+        <v>739</v>
       </c>
       <c r="F788" s="13" t="s">
         <v>814</v>
@@ -45541,13 +45737,13 @@
         <v>0</v>
       </c>
       <c r="N788" s="1" t="s">
-        <v>815</v>
+        <v>1</v>
       </c>
       <c r="O788" s="1" t="s">
         <v>738</v>
       </c>
       <c r="P788" s="7" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="Q788" s="5" t="s">
         <v>738</v>
@@ -45594,13 +45790,13 @@
         <v>0</v>
       </c>
       <c r="N789" s="1" t="s">
-        <v>1</v>
+        <v>815</v>
       </c>
       <c r="O789" s="1" t="s">
         <v>738</v>
       </c>
       <c r="P789" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="Q789" s="5" t="s">
         <v>738</v>
@@ -45647,13 +45843,13 @@
         <v>0</v>
       </c>
       <c r="N790" s="1" t="s">
-        <v>739</v>
+        <v>1</v>
       </c>
       <c r="O790" s="1" t="s">
         <v>738</v>
       </c>
       <c r="P790" s="7" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="Q790" s="5" t="s">
         <v>738</v>
@@ -45700,13 +45896,13 @@
         <v>0</v>
       </c>
       <c r="N791" s="1" t="s">
-        <v>815</v>
+        <v>739</v>
       </c>
       <c r="O791" s="1" t="s">
         <v>738</v>
       </c>
       <c r="P791" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="Q791" s="5" t="s">
         <v>738</v>
@@ -45753,13 +45949,13 @@
         <v>0</v>
       </c>
       <c r="N792" s="1" t="s">
-        <v>1</v>
+        <v>815</v>
       </c>
       <c r="O792" s="1" t="s">
         <v>738</v>
       </c>
       <c r="P792" s="7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="Q792" s="5" t="s">
         <v>738</v>
@@ -45812,10 +46008,10 @@
         <v>738</v>
       </c>
       <c r="P793" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="Q793" s="5" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="794" spans="1:17" x14ac:dyDescent="0.3">
@@ -45865,7 +46061,7 @@
         <v>738</v>
       </c>
       <c r="P794" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="Q794" s="5" t="s">
         <v>737</v>
@@ -45915,10 +46111,10 @@
         <v>1</v>
       </c>
       <c r="O795" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="P795" s="7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="Q795" s="5" t="s">
         <v>737</v>
@@ -45971,7 +46167,7 @@
         <v>737</v>
       </c>
       <c r="P796" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="Q796" s="5" t="s">
         <v>737</v>
@@ -46024,7 +46220,7 @@
         <v>737</v>
       </c>
       <c r="P797" s="7" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="Q797" s="5" t="s">
         <v>737</v>
@@ -46077,7 +46273,7 @@
         <v>737</v>
       </c>
       <c r="P798" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="Q798" s="5" t="s">
         <v>737</v>
@@ -46127,10 +46323,10 @@
         <v>1</v>
       </c>
       <c r="O799" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="P799" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="Q799" s="5" t="s">
         <v>737</v>
@@ -46183,9 +46379,62 @@
         <v>738</v>
       </c>
       <c r="P800" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="Q800" s="5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="801" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A801" s="12" t="s">
+        <v>814</v>
+      </c>
+      <c r="B801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="C801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="D801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="E801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="F801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="G801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="H801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="I801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="J801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="K801" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="L801" s="14" t="s">
+        <v>814</v>
+      </c>
+      <c r="M801" t="s">
+        <v>0</v>
+      </c>
+      <c r="N801" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O801" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="P801" s="7" t="s">
         <v>734</v>
       </c>
-      <c r="Q800" s="5" t="s">
+      <c r="Q801" s="5" t="s">
         <v>737</v>
       </c>
     </row>
@@ -46194,187 +46443,241 @@
     <sortCondition ref="P2:P800"/>
   </sortState>
   <dataConsolidate/>
-  <conditionalFormatting sqref="P2:P734 A238:C249 D203:F212 A250:I800 D213:I249">
-    <cfRule type="cellIs" dxfId="49" priority="60" operator="equal">
+  <conditionalFormatting sqref="P2:P734 A238:C249 D203:F212 A250:I785 D213:I249 A787:I801">
+    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1 I1 F1 C238:C1048576 F203:F1048576 I213:I1048576">
-    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
+  <conditionalFormatting sqref="C1 I1 F1 C238:C785 F203:F785 I213:I785 I787:I1048576 F787:F1048576 C787:C1048576">
+    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1 E1 B1 B238:B1048576 E203:E1048576 H213:H1048576">
-    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
+  <conditionalFormatting sqref="H1 E1 B1 B238:B785 E203:E785 H213:H785 H787:H1048576 E787:E1048576 B787:B1048576">
+    <cfRule type="cellIs" dxfId="71" priority="68" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="69" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J171:L249">
-    <cfRule type="cellIs" dxfId="42" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="66" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1 L171:L249 L801:L1048576">
-    <cfRule type="cellIs" dxfId="40" priority="51" operator="equal">
+  <conditionalFormatting sqref="L1 L171:L249 L802:L1048576">
+    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1 K171:K249 K801:K1048576">
-    <cfRule type="cellIs" dxfId="39" priority="47" operator="equal">
+  <conditionalFormatting sqref="K1 K171:K249 K802:K1048576">
+    <cfRule type="cellIs" dxfId="64" priority="61" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="62" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="64" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O800">
-    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
+  <conditionalFormatting sqref="M2:O801">
+    <cfRule type="cellIs" dxfId="60" priority="59" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="54" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I202 B203:C237 G203:I212">
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F202 C2:C237 I2:I212">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="45" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E202 B2:B237 H2:H212">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="41" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="42" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="43" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="44" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L170">
-    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="32" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="33" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L170">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="31" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K170">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="27" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="28" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J250:L800">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+  <conditionalFormatting sqref="J250:L785 J787:L801">
+    <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L250:L800">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+  <conditionalFormatting sqref="L250:L785 L787:L801">
+    <cfRule type="cellIs" dxfId="37" priority="24" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K250:K800">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+  <conditionalFormatting sqref="K250:K785 K787:K801">
+    <cfRule type="cellIs" dxfId="36" priority="20" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="21" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="22" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A203:A237">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q800">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="Q2:Q801">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q800">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="Q2:Q801">
+    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
       <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A786:I786">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C786 F786 I786">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B786 E786 H786">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J786:L786">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L786">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K786">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46386,19 +46689,19 @@
           <x14:formula1>
             <xm:f>__!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1048576 J2:J1048576 G2:G1048576 D2:D1048576 A2:A1048576</xm:sqref>
+          <xm:sqref>M2:M1048576 A2:A1048576 D2:D1048576 G2:G1048576 J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>__!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576 K2:K1048576 B2:B1048576 E2:E1048576 N2:N1048576</xm:sqref>
+          <xm:sqref>N2:N1048576 E2:E1048576 B2:B1048576 K2:K1048576 H2:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>__!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576 L2:L1048576 C2:C1048576 F2:F1048576 O2:O1048576 Q2:Q800</xm:sqref>
+          <xm:sqref>Q2:Q801 O2:O1048576 F2:F1048576 C2:C1048576 L2:L1048576 I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added movies and subtitles.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -3083,77 +3083,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="75">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="65">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3230,9 +3160,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3265,22 +3208,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3981,8 +3911,8 @@
   <dimension ref="A1:Q801"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A767" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P789" sqref="P789"/>
+      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G305" sqref="G305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12997,7 +12927,7 @@
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B171" s="13" t="s">
         <v>814</v>
@@ -13050,7 +12980,7 @@
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B172" s="13" t="s">
         <v>814</v>
@@ -13103,7 +13033,7 @@
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B173" s="13" t="s">
         <v>814</v>
@@ -13156,7 +13086,7 @@
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B174" s="13" t="s">
         <v>814</v>
@@ -13209,7 +13139,7 @@
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B175" s="13" t="s">
         <v>814</v>
@@ -13262,7 +13192,7 @@
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B176" s="13" t="s">
         <v>814</v>
@@ -13315,7 +13245,7 @@
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B177" s="13" t="s">
         <v>814</v>
@@ -13368,7 +13298,7 @@
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B178" s="13" t="s">
         <v>814</v>
@@ -13421,7 +13351,7 @@
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B179" s="13" t="s">
         <v>814</v>
@@ -13474,7 +13404,7 @@
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B180" s="13" t="s">
         <v>814</v>
@@ -13527,7 +13457,7 @@
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B181" s="13" t="s">
         <v>814</v>
@@ -13580,7 +13510,7 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B182" s="13" t="s">
         <v>814</v>
@@ -13633,7 +13563,7 @@
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B183" s="13" t="s">
         <v>814</v>
@@ -13686,7 +13616,7 @@
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B184" s="13" t="s">
         <v>814</v>
@@ -13739,7 +13669,7 @@
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B185" s="13" t="s">
         <v>814</v>
@@ -13792,7 +13722,7 @@
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B186" s="13" t="s">
         <v>814</v>
@@ -13845,7 +13775,7 @@
     </row>
     <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B187" s="13" t="s">
         <v>814</v>
@@ -13898,7 +13828,7 @@
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B188" s="13" t="s">
         <v>814</v>
@@ -13951,7 +13881,7 @@
     </row>
     <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B189" s="13" t="s">
         <v>814</v>
@@ -14004,7 +13934,7 @@
     </row>
     <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B190" s="13" t="s">
         <v>814</v>
@@ -14057,7 +13987,7 @@
     </row>
     <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B191" s="13" t="s">
         <v>814</v>
@@ -14110,7 +14040,7 @@
     </row>
     <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B192" s="13" t="s">
         <v>814</v>
@@ -14163,7 +14093,7 @@
     </row>
     <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B193" s="13" t="s">
         <v>814</v>
@@ -14216,7 +14146,7 @@
     </row>
     <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B194" s="13" t="s">
         <v>814</v>
@@ -14269,7 +14199,7 @@
     </row>
     <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B195" s="13" t="s">
         <v>814</v>
@@ -14322,7 +14252,7 @@
     </row>
     <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B196" s="13" t="s">
         <v>814</v>
@@ -14375,7 +14305,7 @@
     </row>
     <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B197" s="13" t="s">
         <v>814</v>
@@ -14428,7 +14358,7 @@
     </row>
     <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B198" s="13" t="s">
         <v>814</v>
@@ -14481,7 +14411,7 @@
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B199" s="13" t="s">
         <v>814</v>
@@ -14534,7 +14464,7 @@
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B200" s="13" t="s">
         <v>814</v>
@@ -14587,7 +14517,7 @@
     </row>
     <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B201" s="13" t="s">
         <v>814</v>
@@ -14640,7 +14570,7 @@
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B202" s="13" t="s">
         <v>814</v>
@@ -20099,7 +20029,7 @@
     </row>
     <row r="305" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A305" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B305" s="13" t="s">
         <v>814</v>
@@ -20152,7 +20082,7 @@
     </row>
     <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" s="12" t="s">
-        <v>814</v>
+        <v>0</v>
       </c>
       <c r="B306" s="13" t="s">
         <v>814</v>
@@ -46444,240 +46374,248 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="P2:P734 A238:C249 D203:F212 A250:I785 D213:I249 A787:I801">
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="77" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1 I1 F1 C238:C785 F203:F785 I213:I785 I787:I1048576 F787:F1048576 C787:C1048576">
-    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="74" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 E1 B1 B238:B785 E203:E785 H213:H785 H787:H1048576 E787:E1048576 B787:B1048576">
-    <cfRule type="cellIs" dxfId="71" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="70" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="71" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="72" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="73" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J171:L249">
-    <cfRule type="cellIs" dxfId="67" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="68" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="69" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1 L171:L249 L802:L1048576">
-    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="67" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1 K171:K249 K802:K1048576">
-    <cfRule type="cellIs" dxfId="64" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O801">
-    <cfRule type="cellIs" dxfId="60" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="61" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="58" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="57" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="59" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:I202 B203:C237 G203:I212">
-    <cfRule type="cellIs" dxfId="53" priority="46" operator="equal">
+  <conditionalFormatting sqref="A2:I170 B203:C237 G203:I212 B171:I202">
+    <cfRule type="cellIs" dxfId="43" priority="48" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="49" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F202 C2:C237 I2:I212">
-    <cfRule type="cellIs" dxfId="51" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E202 B2:B237 H2:H212">
-    <cfRule type="cellIs" dxfId="50" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="44" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L170">
-    <cfRule type="cellIs" dxfId="46" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L170">
-    <cfRule type="cellIs" dxfId="44" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K170">
-    <cfRule type="cellIs" dxfId="43" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J250:L785 J787:L801">
-    <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L250:L785 L787:L801">
-    <cfRule type="cellIs" dxfId="37" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K250:K785 K787:K801">
-    <cfRule type="cellIs" dxfId="36" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A203:A237">
-    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A786:I786">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C786 F786 I786">
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B786 E786 H786">
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J786:L786">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L786">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K786">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A171:A202">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46689,7 +46627,7 @@
           <x14:formula1>
             <xm:f>__!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1048576 A2:A1048576 D2:D1048576 G2:G1048576 J2:J1048576</xm:sqref>
+          <xm:sqref>M2:M1048576 J2:J1048576 D2:D1048576 G2:G1048576 A2:A1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Dots for multiplier. Movies for WiiU.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13620" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13654" uniqueCount="820">
   <si>
     <t>Include</t>
   </si>
@@ -2469,6 +2469,12 @@
   </si>
   <si>
     <t>Art/Title/Categories/Arcade/MessageBoxThin</t>
+  </si>
+  <si>
+    <t>Art/Menu/Dot_Empty</t>
+  </si>
+  <si>
+    <t>Art/Menu/Dot_Full</t>
   </si>
 </sst>
 </file>
@@ -3083,7 +3089,755 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="159">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3908,11 +4662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q801"/>
+  <dimension ref="A1:Q803"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G305" sqref="G305"/>
+      <pane ySplit="1" topLeftCell="A790" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P812" sqref="P812"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46361,10 +47115,116 @@
       <c r="O801" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="P801" s="7" t="s">
+      <c r="P801" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="Q801" s="5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="802" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A802" s="12" t="s">
+        <v>814</v>
+      </c>
+      <c r="B802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="C802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="D802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="E802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="F802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="G802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="H802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="I802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="J802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="K802" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="L802" s="14" t="s">
+        <v>814</v>
+      </c>
+      <c r="M802" t="s">
+        <v>0</v>
+      </c>
+      <c r="N802" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O802" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="P802" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="Q802" s="5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="803" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A803" s="12" t="s">
+        <v>814</v>
+      </c>
+      <c r="B803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="C803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="D803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="E803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="F803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="G803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="H803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="I803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="J803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="K803" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="L803" s="14" t="s">
+        <v>814</v>
+      </c>
+      <c r="M803" t="s">
+        <v>0</v>
+      </c>
+      <c r="N803" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O803" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="P803" s="7" t="s">
         <v>734</v>
       </c>
-      <c r="Q801" s="5" t="s">
+      <c r="Q803" s="5" t="s">
         <v>737</v>
       </c>
     </row>
@@ -46374,248 +47234,436 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="P2:P734 A238:C249 D203:F212 A250:I785 D213:I249 A787:I801">
-    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="124" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="125" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1 I1 F1 C238:C785 F203:F785 I213:I785 I787:I1048576 F787:F1048576 C787:C1048576">
-    <cfRule type="cellIs" dxfId="62" priority="74" operator="equal">
+  <conditionalFormatting sqref="C1 I1 F1 C238:C785 F203:F785 I213:I785 I787:I801 F787:F801 C787:C801 C804:C1048576 F804:F1048576 I804:I1048576">
+    <cfRule type="cellIs" dxfId="156" priority="122" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1 E1 B1 B238:B785 E203:E785 H213:H785 H787:H1048576 E787:E1048576 B787:B1048576">
-    <cfRule type="cellIs" dxfId="61" priority="70" operator="equal">
+  <conditionalFormatting sqref="H1 E1 B1 B238:B785 E203:E785 H213:H785 H787:H801 E787:E801 B787:B801 B804:B1048576 E804:E1048576 H804:H1048576">
+    <cfRule type="cellIs" dxfId="155" priority="118" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="119" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="120" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="121" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J171:L249">
-    <cfRule type="cellIs" dxfId="57" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="116" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="117" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1 L171:L249 L802:L1048576">
-    <cfRule type="cellIs" dxfId="55" priority="67" operator="equal">
+  <conditionalFormatting sqref="L1 L171:L249 L804:L1048576">
+    <cfRule type="cellIs" dxfId="149" priority="115" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1 K171:K249 K802:K1048576">
-    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
+  <conditionalFormatting sqref="K1 K171:K249 K804:K1048576">
+    <cfRule type="cellIs" dxfId="148" priority="111" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="112" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="113" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="114" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O801">
-    <cfRule type="cellIs" dxfId="50" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="109" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="110" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
+  <conditionalFormatting sqref="O1:O801 O804:O1048576">
+    <cfRule type="cellIs" dxfId="142" priority="108" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
+  <conditionalFormatting sqref="N1:N801 N804:N1048576">
+    <cfRule type="cellIs" dxfId="141" priority="104" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="105" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="106" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="107" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I170 B203:C237 G203:I212 B171:I202">
-    <cfRule type="cellIs" dxfId="43" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="96" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="97" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F202 C2:C237 I2:I212">
-    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="95" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E202 B2:B237 H2:H212">
-    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="91" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="92" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="93" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="94" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L170">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="82" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="83" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L170">
-    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="81" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K170">
-    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="77" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="78" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="79" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="80" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J250:L785 J787:L801">
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="75" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="76" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L250:L785 L787:L801">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="74" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K250:K785 K787:K801">
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="70" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="71" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="72" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="73" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A203:A237">
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="68" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="69" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="66" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="67" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="65" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A786:I786">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="63" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="64" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C786 F786 I786">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B786 E786 H786">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="58" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="59" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="60" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="61" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J786:L786">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="56" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="57" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L786">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="55" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K786">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="51" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="52" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="53" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="54" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A171:A202">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="49" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="50" operator="equal">
       <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A802:I802">
+    <cfRule type="cellIs" dxfId="95" priority="47" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="48" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I802 F802 C802">
+    <cfRule type="cellIs" dxfId="91" priority="46" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H802 E802 B802">
+    <cfRule type="cellIs" dxfId="89" priority="42" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="43" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="44" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="45" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M802:O802">
+    <cfRule type="cellIs" dxfId="81" priority="40" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="41" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O802">
+    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N802">
+    <cfRule type="cellIs" dxfId="75" priority="35" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="36" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="37" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="38" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J802:L802">
+    <cfRule type="cellIs" dxfId="67" priority="33" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="34" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L802">
+    <cfRule type="cellIs" dxfId="63" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K802">
+    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="29" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="31" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q802">
+    <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q802">
+    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A803:I803">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I803 F803 C803">
+    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H803 E803 B803">
+    <cfRule type="cellIs" dxfId="41" priority="18" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="19" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M803:O803">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O803">
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N803">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J803:L803">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L803">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K803">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q803">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q803">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46639,7 +47687,7 @@
           <x14:formula1>
             <xm:f>__!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q801 O2:O1048576 F2:F1048576 C2:C1048576 L2:L1048576 I2:I1048576</xm:sqref>
+          <xm:sqref>Q2:Q803 O2:O1048576 F2:F1048576 C2:C1048576 L2:L1048576 I2:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
We now build a list of files for Xbox. Added Credits Adobe Premier Project to repo.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -3089,38 +3089,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="159">
+  <dxfs count="109">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3180,9 +3153,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3215,22 +3201,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3290,41 +3263,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -3341,6 +3279,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3400,41 +3345,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -3451,115 +3361,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3619,26 +3420,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
@@ -3670,171 +3451,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3992,26 +3608,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4665,8 +4261,8 @@
   <dimension ref="A1:Q803"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A790" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P812" sqref="P812"/>
+      <pane ySplit="1" topLeftCell="A679" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M708" sqref="M708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13134,7 +12730,7 @@
         <v>814</v>
       </c>
       <c r="M160" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N160" s="1" t="s">
         <v>1</v>
@@ -13187,7 +12783,7 @@
         <v>814</v>
       </c>
       <c r="M161" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N161" s="1" t="s">
         <v>1</v>
@@ -13240,7 +12836,7 @@
         <v>814</v>
       </c>
       <c r="M162" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N162" s="1" t="s">
         <v>1</v>
@@ -13293,7 +12889,7 @@
         <v>814</v>
       </c>
       <c r="M163" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N163" s="1" t="s">
         <v>1</v>
@@ -13346,7 +12942,7 @@
         <v>814</v>
       </c>
       <c r="M164" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N164" s="1" t="s">
         <v>1</v>
@@ -13399,7 +12995,7 @@
         <v>814</v>
       </c>
       <c r="M165" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N165" s="1" t="s">
         <v>1</v>
@@ -13452,7 +13048,7 @@
         <v>814</v>
       </c>
       <c r="M166" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N166" s="1" t="s">
         <v>1</v>
@@ -13505,7 +13101,7 @@
         <v>814</v>
       </c>
       <c r="M167" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N167" s="1" t="s">
         <v>1</v>
@@ -13611,7 +13207,7 @@
         <v>814</v>
       </c>
       <c r="M169" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N169" s="1" t="s">
         <v>1</v>
@@ -13681,7 +13277,7 @@
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B171" s="13" t="s">
         <v>814</v>
@@ -13734,7 +13330,7 @@
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B172" s="13" t="s">
         <v>814</v>
@@ -13787,7 +13383,7 @@
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B173" s="13" t="s">
         <v>814</v>
@@ -13840,7 +13436,7 @@
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B174" s="13" t="s">
         <v>814</v>
@@ -13893,7 +13489,7 @@
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B175" s="13" t="s">
         <v>814</v>
@@ -13946,7 +13542,7 @@
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B176" s="13" t="s">
         <v>814</v>
@@ -13999,7 +13595,7 @@
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B177" s="13" t="s">
         <v>814</v>
@@ -14052,7 +13648,7 @@
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B178" s="13" t="s">
         <v>814</v>
@@ -14105,7 +13701,7 @@
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B179" s="13" t="s">
         <v>814</v>
@@ -14158,7 +13754,7 @@
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B180" s="13" t="s">
         <v>814</v>
@@ -14211,7 +13807,7 @@
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B181" s="13" t="s">
         <v>814</v>
@@ -14264,7 +13860,7 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B182" s="13" t="s">
         <v>814</v>
@@ -14317,7 +13913,7 @@
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B183" s="13" t="s">
         <v>814</v>
@@ -14370,7 +13966,7 @@
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B184" s="13" t="s">
         <v>814</v>
@@ -14423,7 +14019,7 @@
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B185" s="13" t="s">
         <v>814</v>
@@ -14476,7 +14072,7 @@
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B186" s="13" t="s">
         <v>814</v>
@@ -14529,7 +14125,7 @@
     </row>
     <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B187" s="13" t="s">
         <v>814</v>
@@ -14582,7 +14178,7 @@
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B188" s="13" t="s">
         <v>814</v>
@@ -14635,7 +14231,7 @@
     </row>
     <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B189" s="13" t="s">
         <v>814</v>
@@ -14688,7 +14284,7 @@
     </row>
     <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B190" s="13" t="s">
         <v>814</v>
@@ -14741,7 +14337,7 @@
     </row>
     <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B191" s="13" t="s">
         <v>814</v>
@@ -14794,7 +14390,7 @@
     </row>
     <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B192" s="13" t="s">
         <v>814</v>
@@ -14847,7 +14443,7 @@
     </row>
     <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B193" s="13" t="s">
         <v>814</v>
@@ -14900,7 +14496,7 @@
     </row>
     <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B194" s="13" t="s">
         <v>814</v>
@@ -14953,7 +14549,7 @@
     </row>
     <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B195" s="13" t="s">
         <v>814</v>
@@ -15006,7 +14602,7 @@
     </row>
     <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B196" s="13" t="s">
         <v>814</v>
@@ -15059,7 +14655,7 @@
     </row>
     <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B197" s="13" t="s">
         <v>814</v>
@@ -15112,7 +14708,7 @@
     </row>
     <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B198" s="13" t="s">
         <v>814</v>
@@ -15165,7 +14761,7 @@
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B199" s="13" t="s">
         <v>814</v>
@@ -15218,7 +14814,7 @@
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B200" s="13" t="s">
         <v>814</v>
@@ -15271,7 +14867,7 @@
     </row>
     <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B201" s="13" t="s">
         <v>814</v>
@@ -15324,7 +14920,7 @@
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B202" s="13" t="s">
         <v>814</v>
@@ -15377,7 +14973,7 @@
     </row>
     <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B203" s="13" t="s">
         <v>814</v>
@@ -15430,7 +15026,7 @@
     </row>
     <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B204" s="13" t="s">
         <v>814</v>
@@ -15483,7 +15079,7 @@
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B205" s="13" t="s">
         <v>814</v>
@@ -15536,7 +15132,7 @@
     </row>
     <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B206" s="13" t="s">
         <v>814</v>
@@ -15589,7 +15185,7 @@
     </row>
     <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B207" s="13" t="s">
         <v>814</v>
@@ -15642,7 +15238,7 @@
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B208" s="13" t="s">
         <v>814</v>
@@ -15695,7 +15291,7 @@
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B209" s="13" t="s">
         <v>814</v>
@@ -15748,7 +15344,7 @@
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B210" s="13" t="s">
         <v>814</v>
@@ -15801,7 +15397,7 @@
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B211" s="13" t="s">
         <v>814</v>
@@ -15854,7 +15450,7 @@
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B212" s="13" t="s">
         <v>814</v>
@@ -15907,7 +15503,7 @@
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B213" s="13" t="s">
         <v>814</v>
@@ -15960,7 +15556,7 @@
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B214" s="13" t="s">
         <v>814</v>
@@ -16013,7 +15609,7 @@
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B215" s="13" t="s">
         <v>814</v>
@@ -16066,7 +15662,7 @@
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B216" s="13" t="s">
         <v>814</v>
@@ -16119,7 +15715,7 @@
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B217" s="13" t="s">
         <v>814</v>
@@ -16172,7 +15768,7 @@
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B218" s="13" t="s">
         <v>814</v>
@@ -16225,7 +15821,7 @@
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B219" s="13" t="s">
         <v>814</v>
@@ -16278,7 +15874,7 @@
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B220" s="13" t="s">
         <v>814</v>
@@ -16331,7 +15927,7 @@
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B221" s="13" t="s">
         <v>814</v>
@@ -16384,7 +15980,7 @@
     </row>
     <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B222" s="13" t="s">
         <v>814</v>
@@ -16437,7 +16033,7 @@
     </row>
     <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B223" s="13" t="s">
         <v>814</v>
@@ -16490,7 +16086,7 @@
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B224" s="13" t="s">
         <v>814</v>
@@ -16543,7 +16139,7 @@
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B225" s="13" t="s">
         <v>814</v>
@@ -16596,7 +16192,7 @@
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B226" s="13" t="s">
         <v>814</v>
@@ -16649,7 +16245,7 @@
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B227" s="13" t="s">
         <v>814</v>
@@ -16702,7 +16298,7 @@
     </row>
     <row r="228" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A228" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B228" s="13" t="s">
         <v>814</v>
@@ -16755,7 +16351,7 @@
     </row>
     <row r="229" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A229" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B229" s="13" t="s">
         <v>814</v>
@@ -16808,7 +16404,7 @@
     </row>
     <row r="230" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A230" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B230" s="13" t="s">
         <v>814</v>
@@ -16861,7 +16457,7 @@
     </row>
     <row r="231" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A231" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B231" s="13" t="s">
         <v>814</v>
@@ -16914,7 +16510,7 @@
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A232" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B232" s="13" t="s">
         <v>814</v>
@@ -16967,7 +16563,7 @@
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A233" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B233" s="13" t="s">
         <v>814</v>
@@ -17020,7 +16616,7 @@
     </row>
     <row r="234" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A234" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B234" s="13" t="s">
         <v>814</v>
@@ -17073,7 +16669,7 @@
     </row>
     <row r="235" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A235" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B235" s="13" t="s">
         <v>814</v>
@@ -17126,7 +16722,7 @@
     </row>
     <row r="236" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A236" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B236" s="13" t="s">
         <v>814</v>
@@ -17179,7 +16775,7 @@
     </row>
     <row r="237" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A237" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B237" s="13" t="s">
         <v>814</v>
@@ -20783,7 +20379,7 @@
     </row>
     <row r="305" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A305" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B305" s="13" t="s">
         <v>814</v>
@@ -20836,7 +20432,7 @@
     </row>
     <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" s="12" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="B306" s="13" t="s">
         <v>814</v>
@@ -41118,7 +40714,7 @@
         <v>814</v>
       </c>
       <c r="M688" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N688" s="1" t="s">
         <v>1</v>
@@ -42178,7 +41774,7 @@
         <v>814</v>
       </c>
       <c r="M708" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N708" s="1" t="s">
         <v>1</v>
@@ -42867,7 +42463,7 @@
         <v>814</v>
       </c>
       <c r="M721" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N721" s="1" t="s">
         <v>1</v>
@@ -42973,7 +42569,7 @@
         <v>814</v>
       </c>
       <c r="M723" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N723" s="1" t="s">
         <v>1</v>
@@ -43026,7 +42622,7 @@
         <v>814</v>
       </c>
       <c r="M724" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N724" s="1" t="s">
         <v>1</v>
@@ -43132,7 +42728,7 @@
         <v>814</v>
       </c>
       <c r="M726" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N726" s="1" t="s">
         <v>1</v>
@@ -47234,435 +46830,427 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="P2:P734 A238:C249 D203:F212 A250:I785 D213:I249 A787:I801">
-    <cfRule type="cellIs" dxfId="158" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="124" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="125" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1 I1 F1 C238:C785 F203:F785 I213:I785 I787:I801 F787:F801 C787:C801 C804:C1048576 F804:F1048576 I804:I1048576">
-    <cfRule type="cellIs" dxfId="156" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 E1 B1 B238:B785 E203:E785 H213:H785 H787:H801 E787:E801 B787:B801 B804:B1048576 E804:E1048576 H804:H1048576">
-    <cfRule type="cellIs" dxfId="155" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="118" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="119" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="120" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="121" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J171:L249">
-    <cfRule type="cellIs" dxfId="151" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="116" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="117" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1 L171:L249 L804:L1048576">
-    <cfRule type="cellIs" dxfId="149" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="115" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1 K171:K249 K804:K1048576">
-    <cfRule type="cellIs" dxfId="148" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="111" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="112" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="113" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="114" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O801">
-    <cfRule type="cellIs" dxfId="144" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="109" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="110" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O801 O804:O1048576">
-    <cfRule type="cellIs" dxfId="142" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="108" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N801 N804:N1048576">
-    <cfRule type="cellIs" dxfId="141" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="104" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="105" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="106" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="107" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I170 B203:C237 G203:I212 B171:I202">
-    <cfRule type="cellIs" dxfId="137" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="96" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="97" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F202 C2:C237 I2:I212">
-    <cfRule type="cellIs" dxfId="135" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E202 B2:B237 H2:H212">
-    <cfRule type="cellIs" dxfId="134" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="91" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="92" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="93" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="94" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L170">
-    <cfRule type="cellIs" dxfId="130" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="83" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L170">
-    <cfRule type="cellIs" dxfId="128" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="81" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K170">
-    <cfRule type="cellIs" dxfId="127" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="79" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="80" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J250:L785 J787:L801">
-    <cfRule type="cellIs" dxfId="123" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L250:L785 L787:L801">
-    <cfRule type="cellIs" dxfId="121" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K250:K785 K787:K801">
-    <cfRule type="cellIs" dxfId="120" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A203:A237">
-    <cfRule type="cellIs" dxfId="116" priority="68" operator="equal">
+  <conditionalFormatting sqref="Q2:Q801">
+    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="114" priority="66" operator="equal">
-      <formula>"Include"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="67" operator="equal">
-      <formula>"Exclude"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="112" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A786:I786">
-    <cfRule type="cellIs" dxfId="111" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C786 F786 I786">
-    <cfRule type="cellIs" dxfId="109" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B786 E786 H786">
-    <cfRule type="cellIs" dxfId="108" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J786:L786">
-    <cfRule type="cellIs" dxfId="104" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="56" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L786">
-    <cfRule type="cellIs" dxfId="102" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K786">
-    <cfRule type="cellIs" dxfId="101" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A171:A202">
-    <cfRule type="cellIs" dxfId="97" priority="49" operator="equal">
+  <conditionalFormatting sqref="A171:A237">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A802:I802">
-    <cfRule type="cellIs" dxfId="95" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I802 F802 C802">
-    <cfRule type="cellIs" dxfId="91" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H802 E802 B802">
-    <cfRule type="cellIs" dxfId="89" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M802:O802">
-    <cfRule type="cellIs" dxfId="81" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O802">
-    <cfRule type="cellIs" dxfId="77" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N802">
-    <cfRule type="cellIs" dxfId="75" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J802:L802">
-    <cfRule type="cellIs" dxfId="67" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L802">
-    <cfRule type="cellIs" dxfId="63" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K802">
-    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q802">
-    <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q802">
-    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A803:I803">
-    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I803 F803 C803">
-    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H803 E803 B803">
-    <cfRule type="cellIs" dxfId="41" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M803:O803">
-    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O803">
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N803">
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J803:L803">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L803">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K803">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q803">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q803">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added trademark symbol. Added fake ESRB screen and logo salad. Updated credits with cleaner game footage (final credits!)
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13654" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13671" uniqueCount="821">
   <si>
     <t>Include</t>
   </si>
@@ -2475,6 +2475,9 @@
   </si>
   <si>
     <t>Art/Menu/Dot_Full</t>
+  </si>
+  <si>
+    <t>Art/Title/TradeMarkSymbol</t>
   </si>
 </sst>
 </file>
@@ -3089,7 +3092,391 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="109">
+  <dxfs count="157">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4258,11 +4645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q803"/>
+  <dimension ref="A1:Q804"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A679" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M708" sqref="M708"/>
+      <pane ySplit="1" topLeftCell="A778" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K794" sqref="K794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13101,7 +13488,7 @@
         <v>814</v>
       </c>
       <c r="M167" t="s">
-        <v>735</v>
+        <v>0</v>
       </c>
       <c r="N167" s="1" t="s">
         <v>1</v>
@@ -13154,7 +13541,7 @@
         <v>814</v>
       </c>
       <c r="M168" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N168" s="1" t="s">
         <v>1</v>
@@ -44212,7 +44599,7 @@
         <v>814</v>
       </c>
       <c r="M754" t="s">
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="N754" s="1" t="s">
         <v>1</v>
@@ -46229,13 +46616,13 @@
         <v>0</v>
       </c>
       <c r="N792" s="1" t="s">
-        <v>815</v>
+        <v>1</v>
       </c>
       <c r="O792" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="P792" s="7" t="s">
-        <v>725</v>
+      <c r="P792" s="6" t="s">
+        <v>820</v>
       </c>
       <c r="Q792" s="5" t="s">
         <v>738</v>
@@ -46282,13 +46669,13 @@
         <v>0</v>
       </c>
       <c r="N793" s="1" t="s">
-        <v>1</v>
+        <v>815</v>
       </c>
       <c r="O793" s="1" t="s">
         <v>738</v>
       </c>
       <c r="P793" s="7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="Q793" s="5" t="s">
         <v>738</v>
@@ -46341,10 +46728,10 @@
         <v>738</v>
       </c>
       <c r="P794" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="Q794" s="5" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="795" spans="1:17" x14ac:dyDescent="0.3">
@@ -46394,7 +46781,7 @@
         <v>738</v>
       </c>
       <c r="P795" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="Q795" s="5" t="s">
         <v>737</v>
@@ -46444,10 +46831,10 @@
         <v>1</v>
       </c>
       <c r="O796" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="P796" s="7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="Q796" s="5" t="s">
         <v>737</v>
@@ -46500,7 +46887,7 @@
         <v>737</v>
       </c>
       <c r="P797" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="Q797" s="5" t="s">
         <v>737</v>
@@ -46553,7 +46940,7 @@
         <v>737</v>
       </c>
       <c r="P798" s="7" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="Q798" s="5" t="s">
         <v>737</v>
@@ -46606,7 +46993,7 @@
         <v>737</v>
       </c>
       <c r="P799" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="Q799" s="5" t="s">
         <v>737</v>
@@ -46656,10 +47043,10 @@
         <v>1</v>
       </c>
       <c r="O800" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="P800" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="Q800" s="5" t="s">
         <v>737</v>
@@ -46711,8 +47098,8 @@
       <c r="O801" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="P801" s="6" t="s">
-        <v>818</v>
+      <c r="P801" s="7" t="s">
+        <v>733</v>
       </c>
       <c r="Q801" s="5" t="s">
         <v>737</v>
@@ -46765,7 +47152,7 @@
         <v>738</v>
       </c>
       <c r="P802" s="6" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="Q802" s="5" t="s">
         <v>737</v>
@@ -46817,10 +47204,63 @@
       <c r="O803" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="P803" s="7" t="s">
+      <c r="P803" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="Q803" s="5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="804" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A804" s="12" t="s">
+        <v>814</v>
+      </c>
+      <c r="B804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="C804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="D804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="E804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="F804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="G804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="H804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="I804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="J804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="K804" s="13" t="s">
+        <v>814</v>
+      </c>
+      <c r="L804" s="14" t="s">
+        <v>814</v>
+      </c>
+      <c r="M804" t="s">
+        <v>0</v>
+      </c>
+      <c r="N804" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O804" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="P804" s="7" t="s">
         <v>734</v>
       </c>
-      <c r="Q803" s="5" t="s">
+      <c r="Q804" s="5" t="s">
         <v>737</v>
       </c>
     </row>
@@ -46829,428 +47269,522 @@
     <sortCondition ref="P2:P800"/>
   </sortState>
   <dataConsolidate/>
-  <conditionalFormatting sqref="P2:P734 A238:C249 D203:F212 A250:I785 D213:I249 A787:I801">
-    <cfRule type="cellIs" dxfId="108" priority="124" operator="equal">
+  <conditionalFormatting sqref="P2:P734 A238:C249 D203:F212 A250:I785 D213:I249 A787:I791 A793:I802">
+    <cfRule type="cellIs" dxfId="156" priority="148" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="149" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1 I1 F1 C238:C785 F203:F785 I213:I785 I787:I801 F787:F801 C787:C801 C804:C1048576 F804:F1048576 I804:I1048576">
-    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
+  <conditionalFormatting sqref="C1 I1 F1 C238:C785 F203:F785 I213:I785 I787:I791 F787:F791 C787:C791 C805:C1048576 F805:F1048576 I805:I1048576 C793:C802 F793:F802 I793:I802">
+    <cfRule type="cellIs" dxfId="154" priority="146" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1 E1 B1 B238:B785 E203:E785 H213:H785 H787:H801 E787:E801 B787:B801 B804:B1048576 E804:E1048576 H804:H1048576">
-    <cfRule type="cellIs" dxfId="105" priority="118" operator="equal">
+  <conditionalFormatting sqref="H1 E1 B1 B238:B785 E203:E785 H213:H785 H787:H791 E787:E791 B787:B791 B805:B1048576 E805:E1048576 H805:H1048576 B793:B802 E793:E802 H793:H802">
+    <cfRule type="cellIs" dxfId="153" priority="142" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="143" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="144" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="145" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J171:L249">
-    <cfRule type="cellIs" dxfId="101" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="140" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="141" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1 L171:L249 L804:L1048576">
-    <cfRule type="cellIs" dxfId="99" priority="115" operator="equal">
+  <conditionalFormatting sqref="L1 L171:L249 L805:L1048576">
+    <cfRule type="cellIs" dxfId="147" priority="139" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1 K171:K249 K804:K1048576">
-    <cfRule type="cellIs" dxfId="98" priority="111" operator="equal">
+  <conditionalFormatting sqref="K1 K171:K249 K805:K1048576">
+    <cfRule type="cellIs" dxfId="146" priority="135" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="136" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="137" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="138" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O801">
-    <cfRule type="cellIs" dxfId="94" priority="109" operator="equal">
+  <conditionalFormatting sqref="M2:O791 M793:O802">
+    <cfRule type="cellIs" dxfId="142" priority="133" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="134" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O801 O804:O1048576">
-    <cfRule type="cellIs" dxfId="92" priority="108" operator="equal">
+  <conditionalFormatting sqref="O1:O791 O805:O1048576 O793:O802">
+    <cfRule type="cellIs" dxfId="140" priority="132" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N801 N804:N1048576">
-    <cfRule type="cellIs" dxfId="91" priority="104" operator="equal">
+  <conditionalFormatting sqref="N1:N791 N805:N1048576 N793:N802">
+    <cfRule type="cellIs" dxfId="139" priority="128" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="129" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="130" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="131" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I170 B203:C237 G203:I212 B171:I202">
-    <cfRule type="cellIs" dxfId="87" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="120" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="121" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F202 C2:C237 I2:I212">
-    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="119" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E202 B2:B237 H2:H212">
-    <cfRule type="cellIs" dxfId="84" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="115" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="116" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="117" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="118" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L170">
-    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="106" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="107" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L170">
-    <cfRule type="cellIs" dxfId="78" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="105" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K170">
-    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="101" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="102" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="103" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="104" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J250:L785 J787:L801">
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
+  <conditionalFormatting sqref="J250:L785 J787:L791 J793:L802">
+    <cfRule type="cellIs" dxfId="121" priority="99" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="100" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L250:L785 L787:L801">
-    <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
+  <conditionalFormatting sqref="L250:L785 L787:L791 L793:L802">
+    <cfRule type="cellIs" dxfId="119" priority="98" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K250:K785 K787:K801">
-    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
+  <conditionalFormatting sqref="K250:K785 K787:K791 K793:K802">
+    <cfRule type="cellIs" dxfId="118" priority="94" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="95" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="96" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="97" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
+  <conditionalFormatting sqref="Q2:Q791 Q793:Q802">
+    <cfRule type="cellIs" dxfId="114" priority="90" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="91" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q801">
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="equal">
+  <conditionalFormatting sqref="Q2:Q791 Q793:Q802">
+    <cfRule type="cellIs" dxfId="112" priority="89" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A786:I786">
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="87" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="88" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C786 F786 I786">
-    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="86" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B786 E786 H786">
-    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="82" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="83" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="84" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="85" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J786:L786">
-    <cfRule type="cellIs" dxfId="56" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="80" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="81" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L786">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="79" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K786">
-    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="75" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="76" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="77" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="78" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A171:A237">
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="73" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="74" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A802:I802">
-    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+  <conditionalFormatting sqref="A803:I803">
+    <cfRule type="cellIs" dxfId="95" priority="71" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
-      <formula>"Exclude"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I802 F802 C802">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H802 E802 B802">
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
-      <formula>"Raw Rgb, no alpha"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
-      <formula>"DXT5"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
-      <formula>"DXT3"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
-      <formula>"DXT1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M802:O802">
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
-      <formula>"Include"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
-      <formula>"Exclude"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O802">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N802">
-    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
-      <formula>"Raw Rgb, no alpha"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
-      <formula>"DXT5"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
-      <formula>"DXT3"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
-      <formula>"DXT1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J802:L802">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
-      <formula>"Include"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
-      <formula>"Exclude"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L802">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K802">
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
-      <formula>"Raw Rgb, no alpha"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
-      <formula>"DXT5"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
-      <formula>"DXT3"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
-      <formula>"DXT1"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q802">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
-      <formula>"Include"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
-      <formula>"Exclude"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q802">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A803:I803">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
-      <formula>"Include"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="72" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I803 F803 C803">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="70" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H803 E803 B803">
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="66" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="67" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="68" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="69" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M803:O803">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="64" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="65" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O803">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="63" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N803">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="59" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="60" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="61" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="62" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J803:L803">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="57" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="58" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L803">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="56" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K803">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="52" operator="equal">
       <formula>"Raw Rgb, no alpha"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="53" operator="equal">
       <formula>"DXT5"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="54" operator="equal">
       <formula>"DXT3"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="55" operator="equal">
       <formula>"DXT1"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q803">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="50" operator="equal">
       <formula>"Include"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="51" operator="equal">
       <formula>"Exclude"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q803">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="49" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A804:I804">
+    <cfRule type="cellIs" dxfId="71" priority="47" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="48" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I804 F804 C804">
+    <cfRule type="cellIs" dxfId="69" priority="46" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H804 E804 B804">
+    <cfRule type="cellIs" dxfId="68" priority="42" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="43" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="44" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="45" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M804:O804">
+    <cfRule type="cellIs" dxfId="64" priority="40" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O804">
+    <cfRule type="cellIs" dxfId="62" priority="39" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N804">
+    <cfRule type="cellIs" dxfId="61" priority="35" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="36" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="38" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J804:L804">
+    <cfRule type="cellIs" dxfId="57" priority="33" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="34" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L804">
+    <cfRule type="cellIs" dxfId="55" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K804">
+    <cfRule type="cellIs" dxfId="54" priority="28" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="29" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="30" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="31" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q804">
+    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q804">
+    <cfRule type="cellIs" dxfId="48" priority="25" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A792:I792">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C792 F792 I792">
+    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B792 E792 H792">
+    <cfRule type="cellIs" dxfId="41" priority="18" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="19" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M792:O792">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O792">
+    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N792">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J792:L792">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L792">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K792">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+      <formula>"Raw Rgb, no alpha"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+      <formula>"DXT5"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"DXT3"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+      <formula>"DXT1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q792">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Include"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"Exclude"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q792">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47263,19 +47797,19 @@
           <x14:formula1>
             <xm:f>__!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1048576 J2:J1048576 D2:D1048576 G2:G1048576 A2:A1048576</xm:sqref>
+          <xm:sqref>A2:A1048576 G2:G1048576 D2:D1048576 J2:J1048576 M2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>__!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N1048576 E2:E1048576 B2:B1048576 K2:K1048576 H2:H1048576</xm:sqref>
+          <xm:sqref>H2:H1048576 K2:K1048576 B2:B1048576 E2:E1048576 N2:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>__!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q803 O2:O1048576 F2:F1048576 C2:C1048576 L2:L1048576 I2:I1048576</xm:sqref>
+          <xm:sqref>I2:I1048576 L2:L1048576 C2:C1048576 F2:F1048576 O2:O1048576 Q2:Q804</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
WiiU has a new campaign sequence.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -4576,8 +4576,8 @@
   <dimension ref="A1:R803"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q222" sqref="Q222"/>
+      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q254" sqref="Q254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8828,7 +8828,7 @@
         <v>733</v>
       </c>
       <c r="P76" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q76" s="7" t="s">
         <v>76</v>
@@ -8884,7 +8884,7 @@
         <v>733</v>
       </c>
       <c r="P77" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q77" s="7" t="s">
         <v>77</v>
@@ -8940,7 +8940,7 @@
         <v>733</v>
       </c>
       <c r="P78" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q78" s="7" t="s">
         <v>78</v>
@@ -8996,7 +8996,7 @@
         <v>733</v>
       </c>
       <c r="P79" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q79" s="7" t="s">
         <v>79</v>
@@ -9052,7 +9052,7 @@
         <v>733</v>
       </c>
       <c r="P80" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q80" s="7" t="s">
         <v>80</v>
@@ -9108,7 +9108,7 @@
         <v>733</v>
       </c>
       <c r="P81" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q81" s="7" t="s">
         <v>81</v>
@@ -9164,7 +9164,7 @@
         <v>733</v>
       </c>
       <c r="P82" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q82" s="7" t="s">
         <v>82</v>
@@ -9220,7 +9220,7 @@
         <v>733</v>
       </c>
       <c r="P83" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q83" s="7" t="s">
         <v>83</v>
@@ -9276,7 +9276,7 @@
         <v>733</v>
       </c>
       <c r="P84" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q84" s="7" t="s">
         <v>84</v>
@@ -9332,7 +9332,7 @@
         <v>733</v>
       </c>
       <c r="P85" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q85" s="7" t="s">
         <v>85</v>
@@ -9388,7 +9388,7 @@
         <v>733</v>
       </c>
       <c r="P86" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q86" s="7" t="s">
         <v>86</v>
@@ -9444,7 +9444,7 @@
         <v>733</v>
       </c>
       <c r="P87" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q87" s="7" t="s">
         <v>87</v>
@@ -9500,7 +9500,7 @@
         <v>733</v>
       </c>
       <c r="P88" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q88" s="7" t="s">
         <v>88</v>
@@ -9556,7 +9556,7 @@
         <v>733</v>
       </c>
       <c r="P89" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q89" s="7" t="s">
         <v>89</v>
@@ -9612,7 +9612,7 @@
         <v>733</v>
       </c>
       <c r="P90" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q90" s="7" t="s">
         <v>90</v>
@@ -9668,7 +9668,7 @@
         <v>733</v>
       </c>
       <c r="P91" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q91" s="7" t="s">
         <v>91</v>
@@ -9724,7 +9724,7 @@
         <v>733</v>
       </c>
       <c r="P92" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q92" s="7" t="s">
         <v>92</v>
@@ -9780,7 +9780,7 @@
         <v>733</v>
       </c>
       <c r="P93" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q93" s="7" t="s">
         <v>93</v>
@@ -9836,7 +9836,7 @@
         <v>733</v>
       </c>
       <c r="P94" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q94" s="7" t="s">
         <v>94</v>
@@ -9892,7 +9892,7 @@
         <v>733</v>
       </c>
       <c r="P95" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q95" s="7" t="s">
         <v>95</v>
@@ -9948,7 +9948,7 @@
         <v>733</v>
       </c>
       <c r="P96" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q96" s="7" t="s">
         <v>96</v>
@@ -10004,7 +10004,7 @@
         <v>733</v>
       </c>
       <c r="P97" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q97" s="7" t="s">
         <v>97</v>
@@ -10060,7 +10060,7 @@
         <v>733</v>
       </c>
       <c r="P98" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q98" s="7" t="s">
         <v>98</v>
@@ -10116,7 +10116,7 @@
         <v>733</v>
       </c>
       <c r="P99" s="15">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="Q99" s="7" t="s">
         <v>99</v>
@@ -45062,7 +45062,7 @@
         <v>733</v>
       </c>
       <c r="P717" s="15">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="Q717" s="7" t="s">
         <v>648</v>

</xml_diff>

<commit_message>
About to rework load order.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -4576,8 +4576,8 @@
   <dimension ref="A1:R803"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q254" sqref="Q254"/>
+      <pane ySplit="1" topLeftCell="A719" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P783" sqref="P783"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48702,7 +48702,7 @@
         <v>733</v>
       </c>
       <c r="P782" s="15">
-        <v>50</v>
+        <v>1.2</v>
       </c>
       <c r="Q782" s="7" t="s">
         <v>713</v>
@@ -49150,7 +49150,7 @@
         <v>733</v>
       </c>
       <c r="P790" s="15">
-        <v>50</v>
+        <v>1.2</v>
       </c>
       <c r="Q790" s="7" t="s">
         <v>720</v>
@@ -49206,7 +49206,7 @@
         <v>733</v>
       </c>
       <c r="P791" s="15">
-        <v>50</v>
+        <v>1.2</v>
       </c>
       <c r="Q791" s="6" t="s">
         <v>815</v>
@@ -49262,7 +49262,7 @@
         <v>733</v>
       </c>
       <c r="P792" s="15">
-        <v>50</v>
+        <v>1.2</v>
       </c>
       <c r="Q792" s="7" t="s">
         <v>721</v>
@@ -49318,7 +49318,7 @@
         <v>733</v>
       </c>
       <c r="P793" s="15">
-        <v>50</v>
+        <v>1.2</v>
       </c>
       <c r="Q793" s="7" t="s">
         <v>722</v>

</xml_diff>

<commit_message>
Build sent to Ubisoft on March 29, 2013.
</commit_message>
<xml_diff>
--- a/Proj.xlsx
+++ b/Proj.xlsx
@@ -4576,8 +4576,8 @@
   <dimension ref="A1:R803"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A719" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P783" sqref="P783"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q366" sqref="Q366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16052,7 +16052,7 @@
         <v>732</v>
       </c>
       <c r="P205" s="15">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="Q205" s="7" t="s">
         <v>202</v>
@@ -16276,7 +16276,7 @@
         <v>732</v>
       </c>
       <c r="P209" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q209" s="7" t="s">
         <v>206</v>
@@ -16332,7 +16332,7 @@
         <v>732</v>
       </c>
       <c r="P210" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q210" s="7" t="s">
         <v>207</v>
@@ -16388,7 +16388,7 @@
         <v>732</v>
       </c>
       <c r="P211" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q211" s="7" t="s">
         <v>208</v>
@@ -16444,7 +16444,7 @@
         <v>732</v>
       </c>
       <c r="P212" s="15">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="Q212" s="7" t="s">
         <v>209</v>
@@ -17116,7 +17116,7 @@
         <v>732</v>
       </c>
       <c r="P224" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q224" s="7" t="s">
         <v>219</v>
@@ -17172,7 +17172,7 @@
         <v>732</v>
       </c>
       <c r="P225" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q225" s="7" t="s">
         <v>220</v>
@@ -17228,7 +17228,7 @@
         <v>732</v>
       </c>
       <c r="P226" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q226" s="7" t="s">
         <v>221</v>
@@ -17844,7 +17844,7 @@
         <v>732</v>
       </c>
       <c r="P237" s="15">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="Q237" s="7" t="s">
         <v>229</v>
@@ -17900,7 +17900,7 @@
         <v>732</v>
       </c>
       <c r="P238" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q238" s="7" t="s">
         <v>230</v>
@@ -18404,7 +18404,7 @@
         <v>732</v>
       </c>
       <c r="P247" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q247" s="7" t="s">
         <v>237</v>
@@ -18460,7 +18460,7 @@
         <v>732</v>
       </c>
       <c r="P248" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q248" s="7" t="s">
         <v>238</v>
@@ -25569,7 +25569,7 @@
         <f>__!$I$1</f>
         <v>1.5</v>
       </c>
-      <c r="Q374" s="7" t="s">
+      <c r="Q374" s="6" t="s">
         <v>357</v>
       </c>
       <c r="R374" s="5" t="s">
@@ -43102,7 +43102,7 @@
         <v>733</v>
       </c>
       <c r="P682" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q682" s="7" t="s">
         <v>614</v>
@@ -43158,7 +43158,7 @@
         <v>733</v>
       </c>
       <c r="P683" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q683" s="7" t="s">
         <v>615</v>
@@ -43214,7 +43214,7 @@
         <v>733</v>
       </c>
       <c r="P684" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q684" s="7" t="s">
         <v>616</v>
@@ -43270,7 +43270,7 @@
         <v>733</v>
       </c>
       <c r="P685" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q685" s="7" t="s">
         <v>617</v>
@@ -43326,7 +43326,7 @@
         <v>733</v>
       </c>
       <c r="P686" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q686" s="7" t="s">
         <v>618</v>
@@ -43382,7 +43382,7 @@
         <v>733</v>
       </c>
       <c r="P687" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q687" s="7" t="s">
         <v>619</v>
@@ -43438,7 +43438,7 @@
         <v>733</v>
       </c>
       <c r="P688" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q688" s="7" t="s">
         <v>620</v>
@@ -43494,7 +43494,7 @@
         <v>733</v>
       </c>
       <c r="P689" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q689" s="7" t="s">
         <v>621</v>
@@ -43550,7 +43550,7 @@
         <v>733</v>
       </c>
       <c r="P690" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q690" s="7" t="s">
         <v>622</v>
@@ -43606,7 +43606,7 @@
         <v>733</v>
       </c>
       <c r="P691" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q691" s="7" t="s">
         <v>623</v>
@@ -43662,7 +43662,7 @@
         <v>733</v>
       </c>
       <c r="P692" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q692" s="7" t="s">
         <v>624</v>
@@ -43718,7 +43718,7 @@
         <v>733</v>
       </c>
       <c r="P693" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q693" s="7" t="s">
         <v>625</v>
@@ -43774,7 +43774,7 @@
         <v>733</v>
       </c>
       <c r="P694" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q694" s="7" t="s">
         <v>626</v>
@@ -43830,7 +43830,7 @@
         <v>733</v>
       </c>
       <c r="P695" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q695" s="7" t="s">
         <v>627</v>
@@ -43886,7 +43886,7 @@
         <v>733</v>
       </c>
       <c r="P696" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q696" s="7" t="s">
         <v>628</v>
@@ -43942,7 +43942,7 @@
         <v>733</v>
       </c>
       <c r="P697" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q697" s="7" t="s">
         <v>629</v>
@@ -43998,7 +43998,7 @@
         <v>733</v>
       </c>
       <c r="P698" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q698" s="7" t="s">
         <v>630</v>
@@ -44054,7 +44054,7 @@
         <v>733</v>
       </c>
       <c r="P699" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q699" s="7" t="s">
         <v>631</v>
@@ -44110,7 +44110,7 @@
         <v>733</v>
       </c>
       <c r="P700" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q700" s="7" t="s">
         <v>632</v>
@@ -44166,7 +44166,7 @@
         <v>733</v>
       </c>
       <c r="P701" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q701" s="7" t="s">
         <v>633</v>
@@ -44222,7 +44222,7 @@
         <v>733</v>
       </c>
       <c r="P702" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q702" s="7" t="s">
         <v>634</v>
@@ -44278,7 +44278,7 @@
         <v>733</v>
       </c>
       <c r="P703" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q703" s="7" t="s">
         <v>635</v>
@@ -44334,7 +44334,7 @@
         <v>733</v>
       </c>
       <c r="P704" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q704" s="7" t="s">
         <v>636</v>
@@ -44390,7 +44390,7 @@
         <v>733</v>
       </c>
       <c r="P705" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q705" s="7" t="s">
         <v>637</v>
@@ -44446,7 +44446,7 @@
         <v>733</v>
       </c>
       <c r="P706" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q706" s="7" t="s">
         <v>638</v>
@@ -44502,7 +44502,7 @@
         <v>733</v>
       </c>
       <c r="P707" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q707" s="7" t="s">
         <v>639</v>
@@ -44558,7 +44558,7 @@
         <v>733</v>
       </c>
       <c r="P708" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q708" s="7" t="s">
         <v>640</v>
@@ -44614,7 +44614,7 @@
         <v>733</v>
       </c>
       <c r="P709" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q709" s="7" t="s">
         <v>641</v>
@@ -44670,7 +44670,7 @@
         <v>733</v>
       </c>
       <c r="P710" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q710" s="7" t="s">
         <v>642</v>
@@ -44726,7 +44726,7 @@
         <v>733</v>
       </c>
       <c r="P711" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q711" s="7" t="s">
         <v>613</v>
@@ -44782,7 +44782,7 @@
         <v>733</v>
       </c>
       <c r="P712" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q712" s="7" t="s">
         <v>643</v>
@@ -44838,7 +44838,7 @@
         <v>733</v>
       </c>
       <c r="P713" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q713" s="7" t="s">
         <v>644</v>
@@ -44894,7 +44894,7 @@
         <v>733</v>
       </c>
       <c r="P714" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q714" s="7" t="s">
         <v>645</v>
@@ -45118,7 +45118,7 @@
         <v>733</v>
       </c>
       <c r="P718" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q718" s="7" t="s">
         <v>649</v>
@@ -45174,7 +45174,7 @@
         <v>733</v>
       </c>
       <c r="P719" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q719" s="7" t="s">
         <v>650</v>
@@ -45230,7 +45230,7 @@
         <v>733</v>
       </c>
       <c r="P720" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q720" s="7" t="s">
         <v>651</v>
@@ -45286,7 +45286,7 @@
         <v>733</v>
       </c>
       <c r="P721" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q721" s="7" t="s">
         <v>652</v>
@@ -45342,7 +45342,7 @@
         <v>733</v>
       </c>
       <c r="P722" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q722" s="7" t="s">
         <v>653</v>
@@ -45398,7 +45398,7 @@
         <v>733</v>
       </c>
       <c r="P723" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q723" s="7" t="s">
         <v>654</v>
@@ -45454,7 +45454,7 @@
         <v>733</v>
       </c>
       <c r="P724" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q724" s="7" t="s">
         <v>655</v>
@@ -45510,7 +45510,7 @@
         <v>733</v>
       </c>
       <c r="P725" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q725" s="7" t="s">
         <v>656</v>
@@ -45566,7 +45566,7 @@
         <v>733</v>
       </c>
       <c r="P726" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q726" s="7" t="s">
         <v>657</v>
@@ -45622,7 +45622,7 @@
         <v>733</v>
       </c>
       <c r="P727" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q727" s="7" t="s">
         <v>658</v>
@@ -45678,7 +45678,7 @@
         <v>733</v>
       </c>
       <c r="P728" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q728" s="7" t="s">
         <v>659</v>
@@ -45734,7 +45734,7 @@
         <v>733</v>
       </c>
       <c r="P729" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q729" s="7" t="s">
         <v>660</v>
@@ -45790,7 +45790,7 @@
         <v>733</v>
       </c>
       <c r="P730" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q730" s="7" t="s">
         <v>661</v>
@@ -45846,7 +45846,7 @@
         <v>733</v>
       </c>
       <c r="P731" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q731" s="7" t="s">
         <v>662</v>
@@ -45958,7 +45958,7 @@
         <v>733</v>
       </c>
       <c r="P733" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q733" s="7" t="s">
         <v>664</v>
@@ -46014,7 +46014,7 @@
         <v>733</v>
       </c>
       <c r="P734" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q734" s="7" t="s">
         <v>665</v>
@@ -46070,7 +46070,7 @@
         <v>733</v>
       </c>
       <c r="P735" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q735" s="7" t="s">
         <v>666</v>
@@ -46126,7 +46126,7 @@
         <v>733</v>
       </c>
       <c r="P736" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q736" s="7" t="s">
         <v>667</v>
@@ -46182,7 +46182,7 @@
         <v>733</v>
       </c>
       <c r="P737" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q737" s="7" t="s">
         <v>668</v>
@@ -46238,7 +46238,7 @@
         <v>733</v>
       </c>
       <c r="P738" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q738" s="7" t="s">
         <v>669</v>
@@ -46294,7 +46294,7 @@
         <v>733</v>
       </c>
       <c r="P739" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q739" s="7" t="s">
         <v>670</v>
@@ -46350,7 +46350,7 @@
         <v>733</v>
       </c>
       <c r="P740" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q740" s="7" t="s">
         <v>671</v>
@@ -46406,7 +46406,7 @@
         <v>733</v>
       </c>
       <c r="P741" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q741" s="7" t="s">
         <v>672</v>
@@ -46462,7 +46462,7 @@
         <v>733</v>
       </c>
       <c r="P742" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q742" s="7" t="s">
         <v>673</v>
@@ -46518,7 +46518,7 @@
         <v>733</v>
       </c>
       <c r="P743" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q743" s="7" t="s">
         <v>674</v>
@@ -46574,7 +46574,7 @@
         <v>733</v>
       </c>
       <c r="P744" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q744" s="7" t="s">
         <v>675</v>
@@ -46630,7 +46630,7 @@
         <v>733</v>
       </c>
       <c r="P745" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q745" s="7" t="s">
         <v>676</v>
@@ -46686,7 +46686,7 @@
         <v>733</v>
       </c>
       <c r="P746" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q746" s="7" t="s">
         <v>677</v>
@@ -47302,7 +47302,7 @@
         <v>733</v>
       </c>
       <c r="P757" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q757" s="7" t="s">
         <v>688</v>
@@ -47358,7 +47358,7 @@
         <v>733</v>
       </c>
       <c r="P758" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q758" s="7" t="s">
         <v>689</v>
@@ -47414,7 +47414,7 @@
         <v>733</v>
       </c>
       <c r="P759" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q759" s="7" t="s">
         <v>690</v>
@@ -47470,7 +47470,7 @@
         <v>733</v>
       </c>
       <c r="P760" s="15">
-        <v>50</v>
+        <v>1.31</v>
       </c>
       <c r="Q760" s="7" t="s">
         <v>691</v>
@@ -47694,7 +47694,7 @@
         <v>733</v>
       </c>
       <c r="P764" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q764" s="7" t="s">
         <v>695</v>
@@ -47750,7 +47750,7 @@
         <v>733</v>
       </c>
       <c r="P765" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q765" s="7" t="s">
         <v>696</v>
@@ -47806,7 +47806,7 @@
         <v>733</v>
       </c>
       <c r="P766" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q766" s="7" t="s">
         <v>697</v>
@@ -47862,7 +47862,7 @@
         <v>733</v>
       </c>
       <c r="P767" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q767" s="7" t="s">
         <v>698</v>
@@ -47918,7 +47918,7 @@
         <v>733</v>
       </c>
       <c r="P768" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q768" s="7" t="s">
         <v>699</v>
@@ -47974,7 +47974,7 @@
         <v>733</v>
       </c>
       <c r="P769" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q769" s="7" t="s">
         <v>700</v>
@@ -48030,7 +48030,7 @@
         <v>733</v>
       </c>
       <c r="P770" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q770" s="7" t="s">
         <v>701</v>
@@ -48086,7 +48086,7 @@
         <v>733</v>
       </c>
       <c r="P771" s="15">
-        <v>100</v>
+        <v>1.3</v>
       </c>
       <c r="Q771" s="7" t="s">
         <v>702</v>
@@ -48758,7 +48758,7 @@
         <v>733</v>
       </c>
       <c r="P783" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q783" s="7" t="s">
         <v>714</v>
@@ -48814,7 +48814,7 @@
         <v>733</v>
       </c>
       <c r="P784" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q784" s="6" t="s">
         <v>715</v>
@@ -48870,7 +48870,7 @@
         <v>733</v>
       </c>
       <c r="P785" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q785" s="6" t="s">
         <v>812</v>
@@ -48926,7 +48926,7 @@
         <v>733</v>
       </c>
       <c r="P786" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q786" s="7" t="s">
         <v>716</v>
@@ -48982,7 +48982,7 @@
         <v>733</v>
       </c>
       <c r="P787" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q787" s="7" t="s">
         <v>717</v>
@@ -49038,7 +49038,7 @@
         <v>733</v>
       </c>
       <c r="P788" s="15">
-        <v>50</v>
+        <v>1.3</v>
       </c>
       <c r="Q788" s="7" t="s">
         <v>718</v>

</xml_diff>